<commit_message>
-- Phúc -- Sửa lại phần ngày nhận trong file Phân công.xlsx
</commit_message>
<xml_diff>
--- a/Plan/Phân công.xlsx
+++ b/Plan/Phân công.xlsx
@@ -463,7 +463,7 @@
   <dimension ref="B3:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +489,7 @@
         <v>42071</v>
       </c>
       <c r="C4" s="3">
-        <v>42132</v>
+        <v>42073</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>1</v>

</xml_diff>